<commit_message>
modulo de auditor y reportes
</commit_message>
<xml_diff>
--- a/web/reportes/tracking.xlsx
+++ b/web/reportes/tracking.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3811" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4041" uniqueCount="29">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -64,6 +64,45 @@
   </si>
   <si>
     <t>riesgos elimino al usuario cel</t>
+  </si>
+  <si>
+    <t>riesgos dio de alta a Miguel Sandoval</t>
+  </si>
+  <si>
+    <t>riesgos modifico permisos del usuario riesgos</t>
+  </si>
+  <si>
+    <t>riesgos modifico permisos del usuario Miguel Sandoval</t>
+  </si>
+  <si>
+    <t>riesgos dio de alta a coca</t>
+  </si>
+  <si>
+    <t>riesgos modifico permisos del usuario coca</t>
+  </si>
+  <si>
+    <t>coca</t>
+  </si>
+  <si>
+    <t>coca ingreso al sistema</t>
+  </si>
+  <si>
+    <t>coca salio del sistema</t>
+  </si>
+  <si>
+    <t>riesgos dio de baja al usuario coca</t>
+  </si>
+  <si>
+    <t>riesgos habilito al usuario coca</t>
+  </si>
+  <si>
+    <t>Genero reporte Reporte RC01</t>
+  </si>
+  <si>
+    <t>Genero reporte Reporte ICAP</t>
+  </si>
+  <si>
+    <t>Genero reporte Tracking Log</t>
   </si>
 </sst>
 </file>
@@ -5454,16 +5493,16 @@
     </row>
     <row r="142" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B142" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C142" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D142" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C142" s="16" t="n">
+        <v>41802.97175925926</v>
+      </c>
+      <c r="D142" s="18" t="n">
+        <v>41802.97175925926</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F142" s="10">
         <v>0</v>
@@ -5480,16 +5519,16 @@
     </row>
     <row r="143" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B143" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C143" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D143" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C143" s="16" t="n">
+        <v>41802.973078703704</v>
+      </c>
+      <c r="D143" s="18" t="n">
+        <v>41802.973078703704</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F143" s="10">
         <v>0</v>
@@ -5506,16 +5545,16 @@
     </row>
     <row r="144" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B144" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C144" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D144" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C144" s="16" t="n">
+        <v>41802.98372685185</v>
+      </c>
+      <c r="D144" s="18" t="n">
+        <v>41802.98372685185</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F144" s="10">
         <v>0</v>
@@ -5532,16 +5571,16 @@
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B145" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C145" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D145" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C145" s="16" t="n">
+        <v>41802.9852662037</v>
+      </c>
+      <c r="D145" s="18" t="n">
+        <v>41802.9852662037</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F145" s="10">
         <v>0</v>
@@ -5558,16 +5597,16 @@
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B146" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C146" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D146" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C146" s="16" t="n">
+        <v>41802.98813657407</v>
+      </c>
+      <c r="D146" s="18" t="n">
+        <v>41802.98813657407</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F146" s="10">
         <v>0</v>
@@ -5584,16 +5623,16 @@
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B147" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C147" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D147" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C147" s="16" t="n">
+        <v>41802.99209490741</v>
+      </c>
+      <c r="D147" s="18" t="n">
+        <v>41802.99209490741</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F147" s="10">
         <v>0</v>
@@ -5610,16 +5649,16 @@
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B148" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C148" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D148" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C148" s="16" t="n">
+        <v>41802.996886574074</v>
+      </c>
+      <c r="D148" s="18" t="n">
+        <v>41802.996886574074</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F148" s="10">
         <v>0</v>
@@ -5636,16 +5675,16 @@
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B149" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C149" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D149" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C149" s="16" t="n">
+        <v>41804.51609953704</v>
+      </c>
+      <c r="D149" s="18" t="n">
+        <v>41804.51609953704</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F149" s="10">
         <v>0</v>
@@ -5662,16 +5701,16 @@
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B150" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C150" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D150" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C150" s="16" t="n">
+        <v>41804.524502314816</v>
+      </c>
+      <c r="D150" s="18" t="n">
+        <v>41804.524502314816</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F150" s="10">
         <v>0</v>
@@ -5688,16 +5727,16 @@
     </row>
     <row r="151" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B151" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C151" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D151" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C151" s="16" t="n">
+        <v>41804.52474537037</v>
+      </c>
+      <c r="D151" s="18" t="n">
+        <v>41804.52474537037</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F151" s="10">
         <v>0</v>
@@ -5714,16 +5753,16 @@
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C152" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D152" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C152" s="16" t="n">
+        <v>41804.52670138889</v>
+      </c>
+      <c r="D152" s="18" t="n">
+        <v>41804.52670138889</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F152" s="10">
         <v>0</v>
@@ -5740,16 +5779,16 @@
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B153" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C153" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D153" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C153" s="16" t="n">
+        <v>41804.526967592596</v>
+      </c>
+      <c r="D153" s="18" t="n">
+        <v>41804.526967592596</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F153" s="10">
         <v>0</v>
@@ -5766,16 +5805,16 @@
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B154" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C154" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D154" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C154" s="16" t="n">
+        <v>41804.52890046296</v>
+      </c>
+      <c r="D154" s="18" t="n">
+        <v>41804.52890046296</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F154" s="10">
         <v>0</v>
@@ -5792,16 +5831,16 @@
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B155" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C155" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D155" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C155" s="16" t="n">
+        <v>41806.91587962963</v>
+      </c>
+      <c r="D155" s="18" t="n">
+        <v>41806.91587962963</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F155" s="10">
         <v>0</v>
@@ -5818,16 +5857,16 @@
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B156" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C156" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D156" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C156" s="16" t="n">
+        <v>41806.91914351852</v>
+      </c>
+      <c r="D156" s="18" t="n">
+        <v>41806.91914351852</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F156" s="10">
         <v>0</v>
@@ -5844,16 +5883,16 @@
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B157" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C157" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D157" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C157" s="16" t="n">
+        <v>41806.92680555556</v>
+      </c>
+      <c r="D157" s="18" t="n">
+        <v>41806.92680555556</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F157" s="10">
         <v>0</v>
@@ -5870,16 +5909,16 @@
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B158" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D158" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C158" s="16" t="n">
+        <v>41806.92697916667</v>
+      </c>
+      <c r="D158" s="18" t="n">
+        <v>41806.92697916667</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F158" s="10">
         <v>0</v>
@@ -5896,16 +5935,16 @@
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B159" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C159" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D159" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C159" s="16" t="n">
+        <v>41806.92707175926</v>
+      </c>
+      <c r="D159" s="18" t="n">
+        <v>41806.92707175926</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F159" s="10">
         <v>0</v>
@@ -5922,16 +5961,16 @@
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B160" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C160" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D160" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C160" s="16" t="n">
+        <v>41806.93303240741</v>
+      </c>
+      <c r="D160" s="18" t="n">
+        <v>41806.93303240741</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F160" s="10">
         <v>0</v>
@@ -5948,16 +5987,16 @@
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B161" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D161" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C161" s="16" t="n">
+        <v>41806.93318287037</v>
+      </c>
+      <c r="D161" s="18" t="n">
+        <v>41806.93318287037</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F161" s="10">
         <v>0</v>
@@ -5974,16 +6013,16 @@
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B162" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C162" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D162" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C162" s="16" t="n">
+        <v>41806.93561342593</v>
+      </c>
+      <c r="D162" s="18" t="n">
+        <v>41806.93561342593</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F162" s="10">
         <v>0</v>
@@ -6000,16 +6039,16 @@
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B163" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C163" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D163" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C163" s="16" t="n">
+        <v>41806.93587962963</v>
+      </c>
+      <c r="D163" s="18" t="n">
+        <v>41806.93587962963</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F163" s="10">
         <v>0</v>
@@ -6026,16 +6065,16 @@
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B164" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C164" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D164" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C164" s="16" t="n">
+        <v>41806.93671296296</v>
+      </c>
+      <c r="D164" s="18" t="n">
+        <v>41806.93671296296</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F164" s="10">
         <v>0</v>
@@ -6052,16 +6091,16 @@
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B165" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C165" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D165" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C165" s="16" t="n">
+        <v>41806.94064814815</v>
+      </c>
+      <c r="D165" s="18" t="n">
+        <v>41806.94064814815</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F165" s="10">
         <v>0</v>
@@ -6078,16 +6117,16 @@
     </row>
     <row r="166" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B166" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C166" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D166" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C166" s="16" t="n">
+        <v>41806.94326388889</v>
+      </c>
+      <c r="D166" s="18" t="n">
+        <v>41806.94326388889</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F166" s="10">
         <v>0</v>
@@ -6104,16 +6143,16 @@
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B167" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C167" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D167" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C167" s="16" t="n">
+        <v>41806.9534375</v>
+      </c>
+      <c r="D167" s="18" t="n">
+        <v>41806.9534375</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F167" s="10">
         <v>0</v>
@@ -6130,16 +6169,16 @@
     </row>
     <row r="168" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B168" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C168" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D168" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C168" s="16" t="n">
+        <v>41806.95380787037</v>
+      </c>
+      <c r="D168" s="18" t="n">
+        <v>41806.95380787037</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F168" s="10">
         <v>0</v>
@@ -6156,16 +6195,16 @@
     </row>
     <row r="169" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B169" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C169" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D169" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C169" s="16" t="n">
+        <v>41806.95386574074</v>
+      </c>
+      <c r="D169" s="18" t="n">
+        <v>41806.95386574074</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F169" s="10">
         <v>0</v>
@@ -6182,16 +6221,16 @@
     </row>
     <row r="170" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B170" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C170" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D170" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C170" s="16" t="n">
+        <v>41806.95394675926</v>
+      </c>
+      <c r="D170" s="18" t="n">
+        <v>41806.95394675926</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F170" s="10">
         <v>0</v>
@@ -6208,16 +6247,16 @@
     </row>
     <row r="171" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B171" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C171" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D171" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C171" s="16" t="n">
+        <v>41806.95758101852</v>
+      </c>
+      <c r="D171" s="18" t="n">
+        <v>41806.95758101852</v>
       </c>
       <c r="E171" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F171" s="10">
         <v>0</v>
@@ -6234,16 +6273,16 @@
     </row>
     <row r="172" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B172" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C172" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D172" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C172" s="16" t="n">
+        <v>41806.95767361111</v>
+      </c>
+      <c r="D172" s="18" t="n">
+        <v>41806.95767361111</v>
       </c>
       <c r="E172" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F172" s="10">
         <v>0</v>
@@ -6260,16 +6299,16 @@
     </row>
     <row r="173" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B173" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C173" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D173" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C173" s="16" t="n">
+        <v>41806.95930555555</v>
+      </c>
+      <c r="D173" s="18" t="n">
+        <v>41806.95930555555</v>
       </c>
       <c r="E173" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F173" s="10">
         <v>0</v>
@@ -6286,16 +6325,16 @@
     </row>
     <row r="174" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B174" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C174" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D174" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C174" s="16" t="n">
+        <v>41806.959444444445</v>
+      </c>
+      <c r="D174" s="18" t="n">
+        <v>41806.959444444445</v>
       </c>
       <c r="E174" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F174" s="10">
         <v>0</v>
@@ -6312,16 +6351,16 @@
     </row>
     <row r="175" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B175" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C175" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D175" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C175" s="16" t="n">
+        <v>41806.96302083333</v>
+      </c>
+      <c r="D175" s="18" t="n">
+        <v>41806.96302083333</v>
       </c>
       <c r="E175" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F175" s="10">
         <v>0</v>
@@ -6338,16 +6377,16 @@
     </row>
     <row r="176" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B176" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C176" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D176" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C176" s="16" t="n">
+        <v>41806.964907407404</v>
+      </c>
+      <c r="D176" s="18" t="n">
+        <v>41806.964907407404</v>
       </c>
       <c r="E176" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F176" s="10">
         <v>0</v>
@@ -6364,16 +6403,16 @@
     </row>
     <row r="177" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B177" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C177" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D177" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C177" s="16" t="n">
+        <v>41806.9653125</v>
+      </c>
+      <c r="D177" s="18" t="n">
+        <v>41806.9653125</v>
       </c>
       <c r="E177" s="4" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F177" s="10">
         <v>0</v>
@@ -6390,16 +6429,16 @@
     </row>
     <row r="178" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B178" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C178" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D178" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C178" s="16" t="n">
+        <v>41806.96542824074</v>
+      </c>
+      <c r="D178" s="18" t="n">
+        <v>41806.96542824074</v>
       </c>
       <c r="E178" s="4" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F178" s="10">
         <v>0</v>
@@ -6416,16 +6455,16 @@
     </row>
     <row r="179" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B179" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C179" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D179" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C179" s="16" t="n">
+        <v>41806.96545138889</v>
+      </c>
+      <c r="D179" s="18" t="n">
+        <v>41806.96545138889</v>
       </c>
       <c r="E179" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F179" s="10">
         <v>0</v>
@@ -6442,16 +6481,16 @@
     </row>
     <row r="180" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B180" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C180" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D180" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C180" s="16" t="n">
+        <v>41806.96549768518</v>
+      </c>
+      <c r="D180" s="18" t="n">
+        <v>41806.96549768518</v>
       </c>
       <c r="E180" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F180" s="10">
         <v>0</v>
@@ -6468,16 +6507,16 @@
     </row>
     <row r="181" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B181" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C181" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D181" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C181" s="16" t="n">
+        <v>41806.96561342593</v>
+      </c>
+      <c r="D181" s="18" t="n">
+        <v>41806.96561342593</v>
       </c>
       <c r="E181" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F181" s="10">
         <v>0</v>
@@ -6494,16 +6533,16 @@
     </row>
     <row r="182" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B182" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C182" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D182" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C182" s="16" t="n">
+        <v>41806.9656712963</v>
+      </c>
+      <c r="D182" s="18" t="n">
+        <v>41806.9656712963</v>
       </c>
       <c r="E182" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F182" s="10">
         <v>0</v>
@@ -6520,16 +6559,16 @@
     </row>
     <row r="183" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B183" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C183" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D183" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C183" s="16" t="n">
+        <v>41806.965891203705</v>
+      </c>
+      <c r="D183" s="18" t="n">
+        <v>41806.965891203705</v>
       </c>
       <c r="E183" s="4" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F183" s="10">
         <v>0</v>
@@ -6546,16 +6585,16 @@
     </row>
     <row r="184" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B184" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C184" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D184" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C184" s="16" t="n">
+        <v>41806.96601851852</v>
+      </c>
+      <c r="D184" s="18" t="n">
+        <v>41806.96601851852</v>
       </c>
       <c r="E184" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F184" s="10">
         <v>0</v>
@@ -6572,16 +6611,16 @@
     </row>
     <row r="185" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B185" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C185" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D185" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C185" s="16" t="n">
+        <v>41806.966261574074</v>
+      </c>
+      <c r="D185" s="18" t="n">
+        <v>41806.966261574074</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F185" s="10">
         <v>0</v>
@@ -6598,16 +6637,16 @@
     </row>
     <row r="186" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B186" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C186" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D186" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C186" s="16" t="n">
+        <v>41806.96681712963</v>
+      </c>
+      <c r="D186" s="18" t="n">
+        <v>41806.96681712963</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F186" s="10">
         <v>0</v>
@@ -6624,16 +6663,16 @@
     </row>
     <row r="187" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B187" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C187" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D187" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C187" s="16" t="n">
+        <v>41806.96957175926</v>
+      </c>
+      <c r="D187" s="18" t="n">
+        <v>41806.96957175926</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F187" s="10">
         <v>0</v>
@@ -6650,16 +6689,16 @@
     </row>
     <row r="188" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B188" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C188" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D188" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C188" s="16" t="n">
+        <v>41806.9696875</v>
+      </c>
+      <c r="D188" s="18" t="n">
+        <v>41806.9696875</v>
       </c>
       <c r="E188" s="4" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F188" s="10">
         <v>0</v>
@@ -6676,16 +6715,16 @@
     </row>
     <row r="189" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B189" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C189" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D189" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C189" s="16" t="n">
+        <v>41806.9699537037</v>
+      </c>
+      <c r="D189" s="18" t="n">
+        <v>41806.9699537037</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F189" s="10">
         <v>0</v>
@@ -6702,16 +6741,16 @@
     </row>
     <row r="190" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B190" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C190" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D190" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C190" s="16" t="n">
+        <v>41806.97740740741</v>
+      </c>
+      <c r="D190" s="18" t="n">
+        <v>41806.97740740741</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F190" s="10">
         <v>0</v>
@@ -6728,16 +6767,16 @@
     </row>
     <row r="191" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B191" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C191" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D191" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C191" s="16" t="n">
+        <v>41806.97760416667</v>
+      </c>
+      <c r="D191" s="18" t="n">
+        <v>41806.97760416667</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F191" s="10">
         <v>0</v>
@@ -6754,16 +6793,16 @@
     </row>
     <row r="192" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B192" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C192" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D192" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C192" s="16" t="n">
+        <v>41806.977638888886</v>
+      </c>
+      <c r="D192" s="18" t="n">
+        <v>41806.977638888886</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F192" s="10">
         <v>0</v>
@@ -6780,16 +6819,16 @@
     </row>
     <row r="193" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B193" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C193" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D193" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C193" s="16" t="n">
+        <v>41806.97872685185</v>
+      </c>
+      <c r="D193" s="18" t="n">
+        <v>41806.97872685185</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F193" s="10">
         <v>0</v>
@@ -6806,16 +6845,16 @@
     </row>
     <row r="194" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B194" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C194" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D194" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C194" s="16" t="n">
+        <v>41806.97886574074</v>
+      </c>
+      <c r="D194" s="18" t="n">
+        <v>41806.97886574074</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F194" s="10">
         <v>0</v>
@@ -6832,16 +6871,16 @@
     </row>
     <row r="195" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B195" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C195" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D195" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C195" s="16" t="n">
+        <v>41806.97893518519</v>
+      </c>
+      <c r="D195" s="18" t="n">
+        <v>41806.97893518519</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F195" s="10">
         <v>0</v>
@@ -6858,16 +6897,16 @@
     </row>
     <row r="196" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B196" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C196" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D196" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C196" s="16" t="n">
+        <v>41806.978993055556</v>
+      </c>
+      <c r="D196" s="18" t="n">
+        <v>41806.978993055556</v>
       </c>
       <c r="E196" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F196" s="10">
         <v>0</v>
@@ -6884,16 +6923,16 @@
     </row>
     <row r="197" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B197" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C197" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D197" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C197" s="16" t="n">
+        <v>41806.97902777778</v>
+      </c>
+      <c r="D197" s="18" t="n">
+        <v>41806.97902777778</v>
       </c>
       <c r="E197" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F197" s="10">
         <v>0</v>
@@ -6910,16 +6949,16 @@
     </row>
     <row r="198" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B198" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C198" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D198" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C198" s="16" t="n">
+        <v>41806.97907407407</v>
+      </c>
+      <c r="D198" s="18" t="n">
+        <v>41806.97907407407</v>
       </c>
       <c r="E198" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F198" s="10">
         <v>0</v>
@@ -6936,16 +6975,16 @@
     </row>
     <row r="199" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B199" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C199" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D199" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C199" s="16" t="n">
+        <v>41806.97917824074</v>
+      </c>
+      <c r="D199" s="18" t="n">
+        <v>41806.97917824074</v>
       </c>
       <c r="E199" s="4" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F199" s="10">
         <v>0</v>
@@ -6962,16 +7001,16 @@
     </row>
     <row r="200" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B200" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C200" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D200" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C200" s="16" t="n">
+        <v>41806.97918981482</v>
+      </c>
+      <c r="D200" s="18" t="n">
+        <v>41806.97918981482</v>
       </c>
       <c r="E200" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F200" s="10">
         <v>0</v>
@@ -6988,16 +7027,16 @@
     </row>
     <row r="201" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B201" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C201" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D201" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C201" s="16" t="n">
+        <v>41806.98150462963</v>
+      </c>
+      <c r="D201" s="18" t="n">
+        <v>41806.98150462963</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F201" s="10">
         <v>0</v>
@@ -7014,16 +7053,16 @@
     </row>
     <row r="202" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B202" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C202" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D202" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C202" s="16" t="n">
+        <v>41806.981828703705</v>
+      </c>
+      <c r="D202" s="18" t="n">
+        <v>41806.981828703705</v>
       </c>
       <c r="E202" s="4" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F202" s="10">
         <v>0</v>
@@ -7040,16 +7079,16 @@
     </row>
     <row r="203" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B203" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C203" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D203" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C203" s="16" t="n">
+        <v>41806.981886574074</v>
+      </c>
+      <c r="D203" s="18" t="n">
+        <v>41806.981886574074</v>
       </c>
       <c r="E203" s="4" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F203" s="10">
         <v>0</v>
@@ -7066,16 +7105,16 @@
     </row>
     <row r="204" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B204" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C204" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D204" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C204" s="16" t="n">
+        <v>41806.982152777775</v>
+      </c>
+      <c r="D204" s="18" t="n">
+        <v>41806.982152777775</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F204" s="10">
         <v>0</v>
@@ -7092,16 +7131,16 @@
     </row>
     <row r="205" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B205" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C205" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D205" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C205" s="16" t="n">
+        <v>41806.98974537037</v>
+      </c>
+      <c r="D205" s="18" t="n">
+        <v>41806.98974537037</v>
       </c>
       <c r="E205" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F205" s="10">
         <v>0</v>
@@ -7118,16 +7157,16 @@
     </row>
     <row r="206" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B206" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C206" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D206" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C206" s="16" t="n">
+        <v>41806.9999537037</v>
+      </c>
+      <c r="D206" s="18" t="n">
+        <v>41806.9999537037</v>
       </c>
       <c r="E206" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F206" s="10">
         <v>0</v>
@@ -7144,16 +7183,16 @@
     </row>
     <row r="207" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B207" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C207" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D207" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C207" s="16" t="n">
+        <v>41807.005960648145</v>
+      </c>
+      <c r="D207" s="18" t="n">
+        <v>41807.005960648145</v>
       </c>
       <c r="E207" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F207" s="10">
         <v>0</v>
@@ -7170,16 +7209,16 @@
     </row>
     <row r="208" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B208" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C208" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D208" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C208" s="16" t="n">
+        <v>41807.00616898148</v>
+      </c>
+      <c r="D208" s="18" t="n">
+        <v>41807.00616898148</v>
       </c>
       <c r="E208" s="4" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F208" s="10">
         <v>0</v>
@@ -7196,16 +7235,16 @@
     </row>
     <row r="209" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B209" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C209" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D209" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C209" s="16" t="n">
+        <v>41807.00625</v>
+      </c>
+      <c r="D209" s="18" t="n">
+        <v>41807.00625</v>
       </c>
       <c r="E209" s="4" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F209" s="10">
         <v>0</v>
@@ -7222,16 +7261,16 @@
     </row>
     <row r="210" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B210" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C210" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D210" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C210" s="16" t="n">
+        <v>41807.00628472222</v>
+      </c>
+      <c r="D210" s="18" t="n">
+        <v>41807.00628472222</v>
       </c>
       <c r="E210" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F210" s="10">
         <v>0</v>
@@ -7248,16 +7287,16 @@
     </row>
     <row r="211" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B211" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C211" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D211" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C211" s="16" t="n">
+        <v>41807.00633101852</v>
+      </c>
+      <c r="D211" s="18" t="n">
+        <v>41807.00633101852</v>
       </c>
       <c r="E211" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F211" s="10">
         <v>0</v>
@@ -7274,16 +7313,16 @@
     </row>
     <row r="212" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B212" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C212" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D212" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C212" s="16" t="n">
+        <v>41807.00646990741</v>
+      </c>
+      <c r="D212" s="18" t="n">
+        <v>41807.00646990741</v>
       </c>
       <c r="E212" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F212" s="10">
         <v>0</v>
@@ -7300,16 +7339,16 @@
     </row>
     <row r="213" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B213" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C213" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D213" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C213" s="16" t="n">
+        <v>41807.00885416667</v>
+      </c>
+      <c r="D213" s="18" t="n">
+        <v>41807.00885416667</v>
       </c>
       <c r="E213" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F213" s="10">
         <v>0</v>
@@ -7326,16 +7365,16 @@
     </row>
     <row r="214" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B214" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C214" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D214" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C214" s="16" t="n">
+        <v>41807.00913194445</v>
+      </c>
+      <c r="D214" s="18" t="n">
+        <v>41807.00913194445</v>
       </c>
       <c r="E214" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F214" s="10">
         <v>0</v>
@@ -7352,16 +7391,16 @@
     </row>
     <row r="215" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B215" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C215" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D215" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C215" s="16" t="n">
+        <v>41807.014918981484</v>
+      </c>
+      <c r="D215" s="18" t="n">
+        <v>41807.014918981484</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F215" s="10">
         <v>0</v>
@@ -7378,16 +7417,16 @@
     </row>
     <row r="216" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B216" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C216" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D216" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C216" s="16" t="n">
+        <v>41807.02423611111</v>
+      </c>
+      <c r="D216" s="18" t="n">
+        <v>41807.02423611111</v>
       </c>
       <c r="E216" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F216" s="10">
         <v>0</v>
@@ -7404,16 +7443,16 @@
     </row>
     <row r="217" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B217" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C217" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D217" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C217" s="16" t="n">
+        <v>41807.027083333334</v>
+      </c>
+      <c r="D217" s="18" t="n">
+        <v>41807.027083333334</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F217" s="10">
         <v>0</v>
@@ -7430,16 +7469,16 @@
     </row>
     <row r="218" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B218" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C218" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D218" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C218" s="16" t="n">
+        <v>41807.03873842592</v>
+      </c>
+      <c r="D218" s="18" t="n">
+        <v>41807.03873842592</v>
       </c>
       <c r="E218" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F218" s="10">
         <v>0</v>
@@ -7456,16 +7495,16 @@
     </row>
     <row r="219" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B219" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C219" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D219" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C219" s="16" t="n">
+        <v>41807.04425925926</v>
+      </c>
+      <c r="D219" s="18" t="n">
+        <v>41807.04425925926</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F219" s="10">
         <v>0</v>
@@ -7482,16 +7521,16 @@
     </row>
     <row r="220" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B220" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C220" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D220" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C220" s="16" t="n">
+        <v>41807.04614583333</v>
+      </c>
+      <c r="D220" s="18" t="n">
+        <v>41807.04614583333</v>
       </c>
       <c r="E220" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F220" s="10">
         <v>0</v>
@@ -7508,16 +7547,16 @@
     </row>
     <row r="221" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C221" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D221" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C221" s="16" t="n">
+        <v>41807.0540625</v>
+      </c>
+      <c r="D221" s="18" t="n">
+        <v>41807.0540625</v>
       </c>
       <c r="E221" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F221" s="10">
         <v>0</v>
@@ -7534,16 +7573,16 @@
     </row>
     <row r="222" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B222" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C222" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D222" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C222" s="16" t="n">
+        <v>41807.05454861111</v>
+      </c>
+      <c r="D222" s="18" t="n">
+        <v>41807.05454861111</v>
       </c>
       <c r="E222" s="4" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F222" s="10">
         <v>0</v>
@@ -7560,16 +7599,16 @@
     </row>
     <row r="223" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B223" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C223" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D223" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C223" s="16" t="n">
+        <v>41807.0553125</v>
+      </c>
+      <c r="D223" s="18" t="n">
+        <v>41807.0553125</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F223" s="10">
         <v>0</v>
@@ -7586,16 +7625,16 @@
     </row>
     <row r="224" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B224" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C224" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D224" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C224" s="16" t="n">
+        <v>41807.056550925925</v>
+      </c>
+      <c r="D224" s="18" t="n">
+        <v>41807.056550925925</v>
       </c>
       <c r="E224" s="4" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F224" s="10">
         <v>0</v>
@@ -7612,16 +7651,16 @@
     </row>
     <row r="225" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B225" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C225" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D225" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C225" s="16" t="n">
+        <v>41807.057974537034</v>
+      </c>
+      <c r="D225" s="18" t="n">
+        <v>41807.057974537034</v>
       </c>
       <c r="E225" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F225" s="10">
         <v>0</v>
@@ -7638,16 +7677,16 @@
     </row>
     <row r="226" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C226" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D226" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C226" s="16" t="n">
+        <v>41807.0580787037</v>
+      </c>
+      <c r="D226" s="18" t="n">
+        <v>41807.0580787037</v>
       </c>
       <c r="E226" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F226" s="10">
         <v>0</v>
@@ -7664,16 +7703,16 @@
     </row>
     <row r="227" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B227" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C227" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D227" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C227" s="16" t="n">
+        <v>41807.05868055556</v>
+      </c>
+      <c r="D227" s="18" t="n">
+        <v>41807.05868055556</v>
       </c>
       <c r="E227" s="4" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F227" s="10">
         <v>0</v>
@@ -7690,16 +7729,16 @@
     </row>
     <row r="228" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B228" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C228" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D228" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C228" s="16" t="n">
+        <v>41807.06298611111</v>
+      </c>
+      <c r="D228" s="18" t="n">
+        <v>41807.06298611111</v>
       </c>
       <c r="E228" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F228" s="10">
         <v>0</v>
@@ -7716,16 +7755,16 @@
     </row>
     <row r="229" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B229" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C229" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D229" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C229" s="16" t="n">
+        <v>41807.06392361111</v>
+      </c>
+      <c r="D229" s="18" t="n">
+        <v>41807.06392361111</v>
       </c>
       <c r="E229" s="4" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F229" s="10">
         <v>0</v>
@@ -7742,16 +7781,16 @@
     </row>
     <row r="230" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B230" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C230" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D230" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C230" s="16" t="n">
+        <v>41807.06418981482</v>
+      </c>
+      <c r="D230" s="18" t="n">
+        <v>41807.06418981482</v>
       </c>
       <c r="E230" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F230" s="10">
         <v>0</v>
@@ -7768,16 +7807,16 @@
     </row>
     <row r="231" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B231" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C231" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D231" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C231" s="16" t="n">
+        <v>41807.32502314815</v>
+      </c>
+      <c r="D231" s="18" t="n">
+        <v>41807.32502314815</v>
       </c>
       <c r="E231" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F231" s="10">
         <v>0</v>
@@ -7794,16 +7833,16 @@
     </row>
     <row r="232" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B232" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C232" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D232" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C232" s="16" t="n">
+        <v>41807.879791666666</v>
+      </c>
+      <c r="D232" s="18" t="n">
+        <v>41807.879791666666</v>
       </c>
       <c r="E232" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F232" s="10">
         <v>0</v>
@@ -7820,16 +7859,16 @@
     </row>
     <row r="233" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B233" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C233" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D233" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C233" s="16" t="n">
+        <v>41807.88081018518</v>
+      </c>
+      <c r="D233" s="18" t="n">
+        <v>41807.88081018518</v>
       </c>
       <c r="E233" s="4" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F233" s="10">
         <v>0</v>
@@ -7846,16 +7885,16 @@
     </row>
     <row r="234" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B234" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C234" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D234" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C234" s="16" t="n">
+        <v>41807.88452546296</v>
+      </c>
+      <c r="D234" s="18" t="n">
+        <v>41807.88452546296</v>
       </c>
       <c r="E234" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F234" s="10">
         <v>0</v>
@@ -7872,16 +7911,16 @@
     </row>
     <row r="235" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B235" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C235" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D235" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C235" s="16" t="n">
+        <v>41807.88659722222</v>
+      </c>
+      <c r="D235" s="18" t="n">
+        <v>41807.88659722222</v>
       </c>
       <c r="E235" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F235" s="10">
         <v>0</v>
@@ -7898,16 +7937,16 @@
     </row>
     <row r="236" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B236" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C236" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D236" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C236" s="16" t="n">
+        <v>41807.88744212963</v>
+      </c>
+      <c r="D236" s="18" t="n">
+        <v>41807.88744212963</v>
       </c>
       <c r="E236" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F236" s="10">
         <v>0</v>
@@ -7924,16 +7963,16 @@
     </row>
     <row r="237" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B237" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C237" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D237" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C237" s="16" t="n">
+        <v>41807.88753472222</v>
+      </c>
+      <c r="D237" s="18" t="n">
+        <v>41807.88753472222</v>
       </c>
       <c r="E237" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F237" s="10">
         <v>0</v>
@@ -7950,16 +7989,16 @@
     </row>
     <row r="238" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B238" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C238" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D238" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C238" s="16" t="n">
+        <v>41807.888761574075</v>
+      </c>
+      <c r="D238" s="18" t="n">
+        <v>41807.888761574075</v>
       </c>
       <c r="E238" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F238" s="10">
         <v>0</v>
@@ -7976,16 +8015,16 @@
     </row>
     <row r="239" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B239" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C239" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D239" s="18">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C239" s="16" t="n">
+        <v>41807.907847222225</v>
+      </c>
+      <c r="D239" s="18" t="n">
+        <v>41807.907847222225</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F239" s="10">
         <v>0</v>
@@ -8002,16 +8041,16 @@
     </row>
     <row r="240" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B240" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C240" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D240" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C240" s="16" t="n">
+        <v>41807.90828703704</v>
+      </c>
+      <c r="D240" s="18" t="n">
+        <v>41807.90828703704</v>
       </c>
       <c r="E240" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F240" s="10">
         <v>0</v>
@@ -8028,16 +8067,16 @@
     </row>
     <row r="241" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B241" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C241" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D241" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C241" s="16" t="n">
+        <v>41807.90846064815</v>
+      </c>
+      <c r="D241" s="18" t="n">
+        <v>41807.90846064815</v>
       </c>
       <c r="E241" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F241" s="10">
         <v>0</v>
@@ -8054,16 +8093,16 @@
     </row>
     <row r="242" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B242" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C242" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D242" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C242" s="16" t="n">
+        <v>41807.908530092594</v>
+      </c>
+      <c r="D242" s="18" t="n">
+        <v>41807.908530092594</v>
       </c>
       <c r="E242" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F242" s="10">
         <v>0</v>
@@ -8080,16 +8119,16 @@
     </row>
     <row r="243" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B243" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C243" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D243" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C243" s="16" t="n">
+        <v>41807.92271990741</v>
+      </c>
+      <c r="D243" s="18" t="n">
+        <v>41807.92271990741</v>
       </c>
       <c r="E243" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F243" s="10">
         <v>0</v>
@@ -8106,16 +8145,16 @@
     </row>
     <row r="244" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B244" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C244" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D244" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C244" s="16" t="n">
+        <v>41807.92291666667</v>
+      </c>
+      <c r="D244" s="18" t="n">
+        <v>41807.92291666667</v>
       </c>
       <c r="E244" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F244" s="10">
         <v>0</v>
@@ -8132,16 +8171,16 @@
     </row>
     <row r="245" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B245" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C245" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D245" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C245" s="16" t="n">
+        <v>41807.928761574076</v>
+      </c>
+      <c r="D245" s="18" t="n">
+        <v>41807.928761574076</v>
       </c>
       <c r="E245" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F245" s="10">
         <v>0</v>
@@ -8158,16 +8197,16 @@
     </row>
     <row r="246" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B246" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C246" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D246" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C246" s="16" t="n">
+        <v>41807.928923611114</v>
+      </c>
+      <c r="D246" s="18" t="n">
+        <v>41807.928923611114</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F246" s="10">
         <v>0</v>
@@ -8184,16 +8223,16 @@
     </row>
     <row r="247" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B247" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C247" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D247" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C247" s="16" t="n">
+        <v>41807.93728009259</v>
+      </c>
+      <c r="D247" s="18" t="n">
+        <v>41807.93728009259</v>
       </c>
       <c r="E247" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F247" s="10">
         <v>0</v>
@@ -8210,16 +8249,16 @@
     </row>
     <row r="248" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B248" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C248" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D248" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C248" s="16" t="n">
+        <v>41807.93746527778</v>
+      </c>
+      <c r="D248" s="18" t="n">
+        <v>41807.93746527778</v>
       </c>
       <c r="E248" s="4" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F248" s="10">
         <v>0</v>
@@ -8236,16 +8275,16 @@
     </row>
     <row r="249" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B249" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C249" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D249" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C249" s="16" t="n">
+        <v>41807.94180555556</v>
+      </c>
+      <c r="D249" s="18" t="n">
+        <v>41807.94180555556</v>
       </c>
       <c r="E249" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F249" s="10">
         <v>0</v>
@@ -8262,16 +8301,16 @@
     </row>
     <row r="250" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B250" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C250" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D250" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C250" s="16" t="n">
+        <v>41807.94196759259</v>
+      </c>
+      <c r="D250" s="18" t="n">
+        <v>41807.94196759259</v>
       </c>
       <c r="E250" s="4" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F250" s="10">
         <v>0</v>
@@ -8288,16 +8327,16 @@
     </row>
     <row r="251" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B251" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C251" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D251" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C251" s="16" t="n">
+        <v>41807.94372685185</v>
+      </c>
+      <c r="D251" s="18" t="n">
+        <v>41807.94372685185</v>
       </c>
       <c r="E251" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F251" s="10">
         <v>0</v>
@@ -8314,16 +8353,16 @@
     </row>
     <row r="252" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B252" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C252" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D252" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C252" s="16" t="n">
+        <v>41807.94385416667</v>
+      </c>
+      <c r="D252" s="18" t="n">
+        <v>41807.94385416667</v>
       </c>
       <c r="E252" s="4" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F252" s="10">
         <v>0</v>
@@ -8340,16 +8379,16 @@
     </row>
     <row r="253" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B253" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C253" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D253" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C253" s="16" t="n">
+        <v>41807.94835648148</v>
+      </c>
+      <c r="D253" s="18" t="n">
+        <v>41807.94835648148</v>
       </c>
       <c r="E253" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F253" s="10">
         <v>0</v>
@@ -8366,16 +8405,16 @@
     </row>
     <row r="254" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B254" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C254" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D254" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C254" s="16" t="n">
+        <v>41807.94850694444</v>
+      </c>
+      <c r="D254" s="18" t="n">
+        <v>41807.94850694444</v>
       </c>
       <c r="E254" s="4" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F254" s="10">
         <v>0</v>
@@ -8392,16 +8431,16 @@
     </row>
     <row r="255" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B255" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C255" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D255" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C255" s="16" t="n">
+        <v>41807.95048611111</v>
+      </c>
+      <c r="D255" s="18" t="n">
+        <v>41807.95048611111</v>
       </c>
       <c r="E255" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F255" s="10">
         <v>0</v>
@@ -8418,16 +8457,16 @@
     </row>
     <row r="256" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B256" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C256" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D256" s="18">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C256" s="16" t="n">
+        <v>41807.95065972222</v>
+      </c>
+      <c r="D256" s="18" t="n">
+        <v>41807.95065972222</v>
       </c>
       <c r="E256" s="4" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F256" s="10">
         <v>0</v>

</xml_diff>